<commit_message>
commit on 23/01/2018 at 19:30
</commit_message>
<xml_diff>
--- a/excel/abqRVEinputdeck.xlsx
+++ b/excel/abqRVEinputdeck.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4455" activeTab="1" xr2:uid="{3776EC8A-3462-4102-951F-0B8F87636569}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4455" activeTab="2" xr2:uid="{3776EC8A-3462-4102-951F-0B8F87636569}"/>
   </bookViews>
   <sheets>
     <sheet name="Solvers" sheetId="4" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="87">
   <si>
     <t>NAME</t>
   </si>
@@ -48,9 +48,6 @@
     <t>NUMBER OF CONSTANTS</t>
   </si>
   <si>
-    <t>SI UNIT</t>
-  </si>
-  <si>
     <t>VALUE</t>
   </si>
   <si>
@@ -262,13 +259,56 @@
   </si>
   <si>
     <t>Imperial</t>
+  </si>
+  <si>
+    <t>VARIABLE</t>
+  </si>
+  <si>
+    <t>IS ITERABLE</t>
+  </si>
+  <si>
+    <r>
+      <t>R</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>f</t>
+    </r>
+  </si>
+  <si>
+    <t>DESCRIPTION</t>
+  </si>
+  <si>
+    <t>ITERATION DATA</t>
+  </si>
+  <si>
+    <t>MIN-MAX-STEP</t>
+  </si>
+  <si>
+    <t>LIST</t>
+  </si>
+  <si>
+    <t>MIN</t>
+  </si>
+  <si>
+    <t>MAX</t>
+  </si>
+  <si>
+    <t>STEP</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -281,6 +321,14 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <vertAlign val="subscript"/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -371,10 +419,10 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{165C94B8-F5FB-4520-9C61-CCAA834DC2EF}" name="Table3" displayName="Table3" ref="D2:D31" totalsRowShown="0" dataDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{165C94B8-F5FB-4520-9C61-CCAA834DC2EF}" name="Table3" displayName="Table3" ref="D2:D31" totalsRowShown="0" dataDxfId="1">
   <autoFilter ref="D2:D31" xr:uid="{4151ABB9-8E55-4B2F-8246-E7C33E6A6FCD}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{1DE1F940-065D-4B4D-A03E-6C18830ACE6A}" name="Column1" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{1DE1F940-065D-4B4D-A03E-6C18830ACE6A}" name="Column1" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -395,6 +443,26 @@
   <autoFilter ref="H2:H5" xr:uid="{4025E532-5BDC-4963-A972-C3B625C8AA82}"/>
   <tableColumns count="1">
     <tableColumn id="1" xr3:uid="{04D601D8-B42B-4971-92EA-A0374FD2EF66}" name="Column1"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{6E7C60D3-5979-4454-8510-D5AA7547158A}" name="Table2" displayName="Table2" ref="J3:J5" totalsRowShown="0">
+  <autoFilter ref="J3:J5" xr:uid="{D00E09D6-5F5C-4EA9-A7C5-80D21047C1B3}"/>
+  <tableColumns count="1">
+    <tableColumn id="1" xr3:uid="{4F237714-2F14-4D0E-A0FC-0D954837E015}" name="Column1"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{A5298EFA-56C1-4189-AA53-239A4336B568}" name="Table6" displayName="Table6" ref="L2:L5" totalsRowShown="0">
+  <autoFilter ref="L2:L5" xr:uid="{C548009C-CD74-4B04-BF42-0FEC116DE2C1}"/>
+  <tableColumns count="1">
+    <tableColumn id="1" xr3:uid="{E95B9BA9-8745-4EF1-952D-EC5D1798527D}" name="Column1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -711,8 +779,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F873085C-856B-4D2E-AA74-675FA0329D95}">
   <dimension ref="B2:D3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -724,24 +792,24 @@
   <sheetData>
     <row r="2" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
+        <v>72</v>
+      </c>
+      <c r="C2" t="s">
+        <v>53</v>
+      </c>
+      <c r="D2" t="s">
         <v>73</v>
-      </c>
-      <c r="C2" t="s">
-        <v>54</v>
-      </c>
-      <c r="D2" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -775,15 +843,190 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E354EAE4-2437-403E-8AA1-D274A6E536A3}">
-  <dimension ref="A1"/>
+  <dimension ref="B2:L9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="11.85546875" customWidth="1"/>
+    <col min="3" max="3" width="15.140625" customWidth="1"/>
+    <col min="4" max="4" width="11.85546875" customWidth="1"/>
+    <col min="5" max="5" width="16.42578125" customWidth="1"/>
+    <col min="6" max="6" width="10" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>77</v>
+      </c>
+      <c r="C2" t="s">
+        <v>80</v>
+      </c>
+      <c r="D2" t="s">
+        <v>78</v>
+      </c>
+      <c r="E2" t="s">
+        <v>81</v>
+      </c>
+      <c r="F2" t="s">
+        <v>53</v>
+      </c>
+      <c r="G2" t="s">
+        <v>73</v>
+      </c>
+      <c r="H2" t="s">
+        <v>6</v>
+      </c>
+      <c r="I2" t="s">
+        <v>84</v>
+      </c>
+      <c r="J2" t="s">
+        <v>85</v>
+      </c>
+      <c r="K2" t="s">
+        <v>86</v>
+      </c>
+      <c r="L2" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="3" spans="2:12" ht="18" x14ac:dyDescent="0.35">
+      <c r="B3" t="s">
+        <v>79</v>
+      </c>
+      <c r="D3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E3" t="s">
+        <v>82</v>
+      </c>
+      <c r="F3" t="s">
+        <v>60</v>
+      </c>
+      <c r="G3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="D4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E4" t="s">
+        <v>82</v>
+      </c>
+      <c r="F4" t="s">
+        <v>60</v>
+      </c>
+      <c r="G4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="D5" t="s">
+        <v>23</v>
+      </c>
+      <c r="E5" t="s">
+        <v>82</v>
+      </c>
+      <c r="F5" t="s">
+        <v>60</v>
+      </c>
+      <c r="G5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="D6" t="s">
+        <v>23</v>
+      </c>
+      <c r="E6" t="s">
+        <v>82</v>
+      </c>
+      <c r="F6" t="s">
+        <v>60</v>
+      </c>
+      <c r="G6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="D7" t="s">
+        <v>23</v>
+      </c>
+      <c r="E7" t="s">
+        <v>82</v>
+      </c>
+      <c r="F7" t="s">
+        <v>60</v>
+      </c>
+      <c r="G7" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="D8" t="s">
+        <v>23</v>
+      </c>
+      <c r="E8" t="s">
+        <v>82</v>
+      </c>
+      <c r="F8" t="s">
+        <v>60</v>
+      </c>
+      <c r="G8" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="9" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="D9" t="s">
+        <v>23</v>
+      </c>
+      <c r="E9" t="s">
+        <v>82</v>
+      </c>
+      <c r="F9" t="s">
+        <v>60</v>
+      </c>
+      <c r="G9" t="s">
+        <v>27</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="4">
+        <x14:dataValidation type="list" allowBlank="1" xr:uid="{80199820-B0D2-4B22-A468-AD8CF93939D5}">
+          <x14:formula1>
+            <xm:f>'annex-menus'!$J$4:$J$5</xm:f>
+          </x14:formula1>
+          <xm:sqref>D3:D9</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" xr:uid="{FAADA599-7A6B-4E4F-965A-47381481379C}">
+          <x14:formula1>
+            <xm:f>'annex-menus'!$L$3:$L$5</xm:f>
+          </x14:formula1>
+          <xm:sqref>E3:E9</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1" xr:uid="{8A3394EA-C782-40E4-B892-ABF4F718B56E}">
+          <x14:formula1>
+            <xm:f>'annex-menus'!$F$3:$F$23</xm:f>
+          </x14:formula1>
+          <xm:sqref>F3:F9</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1" xr:uid="{264AA49D-5BB1-458C-AC35-A647904B2193}">
+          <x14:formula1>
+            <xm:f>'annex-menus'!$D$3:$D$31</xm:f>
+          </x14:formula1>
+          <xm:sqref>G3:G9</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -812,7 +1055,7 @@
         <v>2</v>
       </c>
       <c r="D2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E2" t="s">
         <v>3</v>
@@ -821,7 +1064,7 @@
         <v>5</v>
       </c>
       <c r="G2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="2:8" x14ac:dyDescent="0.25">
@@ -832,99 +1075,99 @@
         <v>4</v>
       </c>
       <c r="D3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
       <c r="G4" t="s">
-        <v>6</v>
+        <v>73</v>
       </c>
       <c r="H4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.25">
       <c r="G5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.25">
       <c r="G7" t="s">
-        <v>6</v>
+        <v>73</v>
       </c>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.25">
       <c r="G8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G9" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.25">
       <c r="G10" t="s">
-        <v>6</v>
+        <v>73</v>
       </c>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.25">
       <c r="G11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D12" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G12" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.25">
       <c r="G13" t="s">
-        <v>6</v>
+        <v>73</v>
       </c>
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.25">
       <c r="G14" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="4">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid entry!" error="Check the manual" promptTitle="Type of elastic behavior" prompt="See:_x000a_http://abaqus.software.polimi.it/v2016/books/key/default.htm_x000a_http://abaqus.software.polimi.it/v2016/books/ker/default.htm" xr:uid="{24D5AAE7-4805-47A8-8161-62F93974BEBD}">
           <x14:formula1>
             <xm:f>'annex-menus'!$B$3:$B$11</xm:f>
@@ -943,6 +1186,12 @@
           </x14:formula1>
           <xm:sqref>H4</xm:sqref>
         </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" xr:uid="{8491043E-CE0B-4155-A080-AC397D7B9261}">
+          <x14:formula1>
+            <xm:f>'annex-menus'!$J$4:$J$5</xm:f>
+          </x14:formula1>
+          <xm:sqref>D3 D6 D9 D12</xm:sqref>
+        </x14:dataValidation>
       </x14:dataValidations>
     </ext>
   </extLst>
@@ -951,10 +1200,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6453361E-A457-4BC4-AB4E-AB7D776D7706}">
-  <dimension ref="B2:H31"/>
+  <dimension ref="B2:L31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -963,271 +1212,293 @@
     <col min="4" max="4" width="17.42578125" customWidth="1"/>
     <col min="6" max="6" width="18.5703125" customWidth="1"/>
     <col min="8" max="8" width="15.5703125" customWidth="1"/>
+    <col min="10" max="10" width="11" customWidth="1"/>
+    <col min="12" max="12" width="15.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+      <c r="L2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F3" t="s">
+        <v>54</v>
+      </c>
+      <c r="H3" t="s">
+        <v>74</v>
+      </c>
+      <c r="J3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
         <v>12</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D4" t="s">
         <v>25</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F4" t="s">
         <v>55</v>
       </c>
-      <c r="H3" t="s">
+      <c r="H4" t="s">
+        <v>76</v>
+      </c>
+      <c r="J4" t="s">
+        <v>22</v>
+      </c>
+      <c r="L4" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="5" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" t="s">
+        <v>26</v>
+      </c>
+      <c r="F5" t="s">
+        <v>56</v>
+      </c>
+      <c r="H5" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4" t="s">
-        <v>26</v>
-      </c>
-      <c r="F4" t="s">
-        <v>56</v>
-      </c>
-      <c r="H4" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
+      <c r="J5" t="s">
+        <v>23</v>
+      </c>
+      <c r="L5" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="6" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
         <v>14</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D6" t="s">
         <v>27</v>
       </c>
-      <c r="F5" t="s">
+      <c r="F6" t="s">
         <v>57</v>
       </c>
-      <c r="H5" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B6" t="s">
+    </row>
+    <row r="7" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
         <v>15</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D7" t="s">
         <v>28</v>
       </c>
-      <c r="F6" t="s">
+      <c r="F7" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B7" t="s">
+    <row r="8" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
         <v>16</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D8" t="s">
         <v>29</v>
       </c>
-      <c r="F7" t="s">
+      <c r="F8" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B8" t="s">
+    <row r="9" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
         <v>17</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D9" t="s">
         <v>30</v>
       </c>
-      <c r="F8" t="s">
+      <c r="F9" s="1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B9" t="s">
+    <row r="10" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
         <v>18</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D10" t="s">
         <v>31</v>
       </c>
-      <c r="F9" s="1" t="s">
+      <c r="F10" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="11" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>19</v>
+      </c>
+      <c r="D11" t="s">
+        <v>32</v>
+      </c>
+      <c r="F11" s="1" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
-        <v>19</v>
-      </c>
-      <c r="D10" t="s">
-        <v>32</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B11" t="s">
-        <v>20</v>
-      </c>
-      <c r="D11" t="s">
+    <row r="12" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="D12" t="s">
         <v>33</v>
       </c>
-      <c r="F11" s="1" t="s">
+      <c r="F12" s="1" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="12" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="D12" t="s">
+    <row r="13" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="D13" t="s">
         <v>34</v>
       </c>
-      <c r="F12" s="1" t="s">
+    </row>
+    <row r="14" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="D14" t="s">
+        <v>35</v>
+      </c>
+      <c r="F14" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="13" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="D13" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="14" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="D14" t="s">
+    <row r="15" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="D15" t="s">
         <v>36</v>
       </c>
-      <c r="F14" t="s">
+      <c r="F15" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="15" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="D15" t="s">
+    <row r="16" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="D16" t="s">
         <v>37</v>
       </c>
-      <c r="F15" t="s">
+      <c r="F16" t="s">
         <v>65</v>
-      </c>
-    </row>
-    <row r="16" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="D16" t="s">
-        <v>38</v>
-      </c>
-      <c r="F16" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="17" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D17" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F17" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="18" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D18" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F18" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="19" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D19" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F19" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="20" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D20" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F20" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="21" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D21" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F21" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="22" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D22" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F22" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="23" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D23" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F23" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="24" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D24" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="25" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D25" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="26" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D26" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="27" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D27" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="28" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D28" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="29" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D29" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="30" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D30" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="31" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D31" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
-  <tableParts count="4">
+  <tableParts count="6">
     <tablePart r:id="rId2"/>
     <tablePart r:id="rId3"/>
     <tablePart r:id="rId4"/>
     <tablePart r:id="rId5"/>
+    <tablePart r:id="rId6"/>
+    <tablePart r:id="rId7"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>